<commit_message>
Final version of my presentation and updated delay file
</commit_message>
<xml_diff>
--- a/Delay_Data.xlsx
+++ b/Delay_Data.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diede\Documents\CS4630_MobileComputing\StepCounter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashkan\Google Drive\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4178"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4185"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>Disagree</t>
   </si>
@@ -64,11 +64,44 @@
   <si>
     <t>Average Group Rating</t>
   </si>
+  <si>
+    <t>Strongly Disagree (1)</t>
+  </si>
+  <si>
+    <t>Disagree (2)</t>
+  </si>
+  <si>
+    <t>Neither agree no disagree (3)</t>
+  </si>
+  <si>
+    <t>Agree (4)</t>
+  </si>
+  <si>
+    <t>Strongly Agree (5)</t>
+  </si>
+  <si>
+    <t>200 ms</t>
+  </si>
+  <si>
+    <t>300 ms</t>
+  </si>
+  <si>
+    <t>400 ms</t>
+  </si>
+  <si>
+    <t>450 ms</t>
+  </si>
+  <si>
+    <t>500 ms</t>
+  </si>
+  <si>
+    <t>600 ms</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -115,6 +148,2072 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>200ms Delay</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Strongly Disagree (1)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Disagree (2)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Neither agree no disagree (3)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Agree (4)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Strongly Agree (5)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>300 ms Delay</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>400 ms Delay</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$12:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>450 ms Delay</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$16:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>500 ms DElay</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$20:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>600 ms Delay</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$24:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="493288504"/>
+        <c:axId val="493287328"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="493288504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="493287328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="493287328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Number of votes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="493288504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200">
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet1!$I$3,Sheet1!$I$8,Sheet1!$I$12,Sheet1!$I$16,Sheet1!$I$20,Sheet1!$I$24)</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>200 ms</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300 ms</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400 ms</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>450 ms</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500 ms</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600 ms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$H$3,Sheet1!$H$8,Sheet1!$H$12,Sheet1!$H$16,Sheet1!$H$20,Sheet1!$H$24)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="493922840"/>
+        <c:axId val="166482512"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="493922840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Delay</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="166482512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="166482512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average value </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="493922840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200">
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>18288</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -414,25 +2513,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1328125" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="5" max="5" width="12.53125" customWidth="1"/>
+    <col min="1" max="1" width="53.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -440,21 +2541,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="G3">
         <f>1*1+2*2+1*4</f>
@@ -464,24 +2565,33 @@
         <f>G3/4</f>
         <v>2.25</v>
       </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
       <c r="D4">
         <v>1</v>
       </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -498,12 +2608,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
       <c r="B8">
         <v>3</v>
       </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
       <c r="D8">
         <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
       </c>
       <c r="G8">
         <f>2*3+4</f>
@@ -513,13 +2632,16 @@
         <f>G8/4</f>
         <v>2.5</v>
       </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -536,15 +2658,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
       <c r="D12">
         <v>2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
       </c>
       <c r="G12">
         <f>1+1+2*4</f>
@@ -554,13 +2682,16 @@
         <f>G12/4</f>
         <v>2.5</v>
       </c>
+      <c r="I12" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -577,12 +2708,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
       <c r="C16">
         <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -595,13 +2732,16 @@
         <f>G16/4</f>
         <v>2</v>
       </c>
+      <c r="I16" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -618,15 +2758,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
       <c r="D20">
         <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
       </c>
       <c r="G20">
         <f>2+2+4</f>
@@ -636,13 +2782,16 @@
         <f>G20/4</f>
         <v>2</v>
       </c>
+      <c r="I20" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -659,12 +2808,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
       <c r="B24">
         <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
       </c>
       <c r="G24">
         <f>3+2</f>
@@ -674,8 +2832,12 @@
         <f>G24/4</f>
         <v>1.25</v>
       </c>
+      <c r="I24" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>